<commit_message>
load data almost done
</commit_message>
<xml_diff>
--- a/input/responses/responses_2024-01-09_hard_copies.xlsx
+++ b/input/responses/responses_2024-01-09_hard_copies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthsharedservice.sharepoint.com/sites/sr-ple-ea/analytlead/Statistics and Data Science/Data Science/Products &amp; Projects/20240319_consultation_training/consultation_example/input/responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7554D951-F7B1-44D4-9820-F771DC4A2CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{082FA4C6-56AE-47DD-9AEF-554CA58A3C77}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{7554D951-F7B1-44D4-9820-F771DC4A2CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9398F99E-C815-48BA-AC55-1B7F87E159F8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29835" yWindow="-1065" windowWidth="20805" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>In what capacity are you responding to this survey?</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Please explain your answer_2</t>
+  </si>
+  <si>
+    <t>completed</t>
   </si>
 </sst>
 </file>
@@ -1141,6 +1144,9 @@
       <c r="O2" t="s">
         <v>38</v>
       </c>
+      <c r="Q2" t="s">
+        <v>50</v>
+      </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1187,6 +1193,9 @@
       <c r="O3" t="s">
         <v>42</v>
       </c>
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1238,6 +1247,9 @@
       </c>
       <c r="O4" t="s">
         <v>47</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>50</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1349,25 +1361,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AF14F300012244BA79AC1F66BBF765A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="553212c356cb11e2701639f8ab4feb3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d" xmlns:ns3="7aa07ef2-f4ec-4a8c-98d7-e2e24130d9f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca9dd0b1081054472e26110f86c3e149" ns2:_="" ns3:_="">
     <xsd:import namespace="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
@@ -1578,25 +1571,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BED508B2-A570-4F56-A78C-BA969B70DE9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A2608A2-EE5D-4B6E-BD57-689A58CF73DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF5FC095-C439-4393-A619-473E66D97232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1613,4 +1607,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A2608A2-EE5D-4B6E-BD57-689A58CF73DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BED508B2-A570-4F56-A78C-BA969B70DE9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>